<commit_message>
Fixed UI - I was giving a wrong error. Saying "bookmark error returned" instead of "bookmark - unexpected return (or non-mas build)"
So my UI was wrong! (== instead of ===).

But now I'm totally confused. It says it is a MAS build but it is acting like it is not a MAS build.
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrosen/dev/bookmarkTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5C00BB-309B-1144-B458-CAABF1901BE8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E67B1B-4DB6-F641-8F11-90AB05C9F195}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54460" yWindow="8440" windowWidth="28040" windowHeight="17440" xr2:uid="{433B931A-45DF-3D47-BA1C-2D61C2836698}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Bookmark App Test Results</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>0.1.29x</t>
+  </si>
+  <si>
+    <t>New Certificates - Same results</t>
+  </si>
+  <si>
+    <t>Bogus Provisioning Profile - as expected'</t>
+  </si>
+  <si>
+    <t>NOTE - all bookmark errors up to here were wrong! I *thought* it was giving me an empty string (ie: bookmark error) but it's actually returning [], which either means non-mas build, or unexpected return value.</t>
   </si>
 </sst>
 </file>
@@ -224,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -246,6 +255,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -614,7 +629,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +776,9 @@
       <c r="I6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="K6" s="7" t="s">
         <v>15</v>
       </c>
@@ -776,7 +793,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -792,36 +811,48 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="L8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="N8" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>

</xml_diff>